<commit_message>
Updated NetJSON results and Alibaba results.
Changed Java to use Java bean standard.
Genson doesn't work otherwise, but it has other kind of problems, like failing to deserialize 0.0 as float ;(

Added Alibaba converters for joda time.
</commit_message>
<xml_diff>
--- a/results/result-dotnet-vs-mono-2016.xlsx
+++ b/results/result-dotnet-vs-mono-2016.xlsx
@@ -634,11 +634,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="38595584"/>
-        <c:axId val="38606720"/>
+        <c:axId val="166578432"/>
+        <c:axId val="166830080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="38595584"/>
+        <c:axId val="166578432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -648,7 +648,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38606720"/>
+        <c:crossAx val="166830080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -656,7 +656,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38606720"/>
+        <c:axId val="166830080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -687,7 +687,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38595584"/>
+        <c:crossAx val="166578432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -968,11 +968,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="39532416"/>
-        <c:axId val="39867136"/>
+        <c:axId val="167565184"/>
+        <c:axId val="167566720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39532416"/>
+        <c:axId val="167565184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -982,7 +982,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39867136"/>
+        <c:crossAx val="167566720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -990,7 +990,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39867136"/>
+        <c:axId val="167566720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1020,7 +1020,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39532416"/>
+        <c:crossAx val="167565184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1163,7 +1163,7 @@
                   <c:v>20929.666666666668</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17409.333333333336</c:v>
+                  <c:v>20310.666666666664</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>58389.333333333336</c:v>
@@ -1179,6 +1179,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>70017.333333333343</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>47567.333333333336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1265,7 +1268,7 @@
                   <c:v>31256.333333333339</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>65605.666666666672</c:v>
+                  <c:v>85417.666666666672</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>117716.33333333331</c:v>
@@ -1281,6 +1284,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>49923.666666666664</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>121975.66666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1295,11 +1301,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="40712064"/>
-        <c:axId val="40729216"/>
+        <c:axId val="168052224"/>
+        <c:axId val="168053760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="40712064"/>
+        <c:axId val="168052224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1309,7 +1315,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40729216"/>
+        <c:crossAx val="168053760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1317,7 +1323,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40729216"/>
+        <c:axId val="168053760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1348,7 +1354,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40712064"/>
+        <c:crossAx val="168052224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1491,6 +1497,9 @@
                 <c:pt idx="4">
                   <c:v>6462</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>3304.9999999999995</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>10589.333333333334</c:v>
                 </c:pt>
@@ -1505,6 +1514,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>12954</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6055.666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1590,6 +1602,9 @@
                 <c:pt idx="4">
                   <c:v>7116.3333333333321</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>10630.333333333334</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>16399.333333333336</c:v>
                 </c:pt>
@@ -1604,6 +1619,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>9284.9999999999982</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23440</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1618,11 +1636,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="41005440"/>
-        <c:axId val="41008128"/>
+        <c:axId val="168195200"/>
+        <c:axId val="168196736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41005440"/>
+        <c:axId val="168195200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1632,7 +1650,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41008128"/>
+        <c:crossAx val="168196736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1640,7 +1658,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41008128"/>
+        <c:axId val="168196736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1671,7 +1689,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41005440"/>
+        <c:crossAx val="168195200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1814,6 +1832,9 @@
                 <c:pt idx="4">
                   <c:v>177506.66666666669</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>105545</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>403286</c:v>
                 </c:pt>
@@ -1828,6 +1849,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>440149.33333333326</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>216158.33333333334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1913,6 +1937,9 @@
                 <c:pt idx="4">
                   <c:v>156733</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>346493.66666666663</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>369393.66666666663</c:v>
                 </c:pt>
@@ -1927,6 +1954,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>328337</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>867790.66666666651</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1941,11 +1971,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="42167296"/>
-        <c:axId val="42377984"/>
+        <c:axId val="168293120"/>
+        <c:axId val="168294656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="42167296"/>
+        <c:axId val="168293120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1955,7 +1985,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42377984"/>
+        <c:crossAx val="168294656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1963,7 +1993,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42377984"/>
+        <c:axId val="168294656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1994,7 +2024,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42167296"/>
+        <c:crossAx val="168293120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2239,11 +2269,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="130567552"/>
-        <c:axId val="130843776"/>
+        <c:axId val="168370560"/>
+        <c:axId val="168372096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="130567552"/>
+        <c:axId val="168370560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2253,7 +2283,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130843776"/>
+        <c:crossAx val="168372096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2261,7 +2291,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="130843776"/>
+        <c:axId val="168372096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2291,7 +2321,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130567552"/>
+        <c:crossAx val="168370560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2944,7 +2974,7 @@
   <dimension ref="B1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3674,7 +3704,7 @@
         <v>7991.333333333333</v>
       </c>
       <c r="H22" s="1">
-        <v>8192.3333333333339</v>
+        <v>7893.666666666667</v>
       </c>
       <c r="I22" s="1">
         <v>33303.333333333336</v>
@@ -3692,7 +3722,7 @@
         <v>34675.333333333336</v>
       </c>
       <c r="N22" s="1">
-        <v>35209.666666666664</v>
+        <v>35073.333333333336</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -3718,7 +3748,7 @@
         <v>20929.666666666668</v>
       </c>
       <c r="H23" s="1">
-        <v>17409.333333333336</v>
+        <v>20310.666666666664</v>
       </c>
       <c r="I23" s="1">
         <v>58389.333333333336</v>
@@ -3735,7 +3765,9 @@
       <c r="M23" s="1">
         <v>70017.333333333343</v>
       </c>
-      <c r="N23" s="1"/>
+      <c r="N23" s="1">
+        <v>47567.333333333336</v>
+      </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
@@ -3760,7 +3792,7 @@
         <v>31256.333333333339</v>
       </c>
       <c r="H24" s="1">
-        <v>65605.666666666672</v>
+        <v>85417.666666666672</v>
       </c>
       <c r="I24" s="1">
         <v>117716.33333333331</v>
@@ -3777,7 +3809,9 @@
       <c r="M24" s="1">
         <v>49923.666666666664</v>
       </c>
-      <c r="N24" s="1"/>
+      <c r="N24" s="1">
+        <v>121975.66666666666</v>
+      </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
@@ -3802,7 +3836,7 @@
         <v>60177.333333333336</v>
       </c>
       <c r="H25" s="1">
-        <v>91207.333333333328</v>
+        <v>113622</v>
       </c>
       <c r="I25" s="1">
         <v>209409</v>
@@ -3819,7 +3853,9 @@
       <c r="M25" s="1">
         <v>154616.33333333334</v>
       </c>
-      <c r="N25" s="1"/>
+      <c r="N25" s="1">
+        <v>204616.33333333334</v>
+      </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
@@ -3985,7 +4021,9 @@
       <c r="G22" s="1">
         <v>2572.3333333333335</v>
       </c>
-      <c r="H22" s="1"/>
+      <c r="H22" s="1">
+        <v>2556.3333333333335</v>
+      </c>
       <c r="I22" s="1">
         <v>1614</v>
       </c>
@@ -4001,7 +4039,9 @@
       <c r="M22" s="1">
         <v>1631.3333333333333</v>
       </c>
-      <c r="N22" s="1"/>
+      <c r="N22" s="1">
+        <v>1680.3333333333333</v>
+      </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
@@ -4025,7 +4065,9 @@
       <c r="G23" s="1">
         <v>6462</v>
       </c>
-      <c r="H23" s="1"/>
+      <c r="H23" s="1">
+        <v>3304.9999999999995</v>
+      </c>
       <c r="I23" s="1">
         <v>10589.333333333334</v>
       </c>
@@ -4041,7 +4083,9 @@
       <c r="M23" s="1">
         <v>12954</v>
       </c>
-      <c r="N23" s="1"/>
+      <c r="N23" s="1">
+        <v>6055.666666666667</v>
+      </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
@@ -4065,7 +4109,9 @@
       <c r="G24" s="1">
         <v>7116.3333333333321</v>
       </c>
-      <c r="H24" s="1"/>
+      <c r="H24" s="1">
+        <v>10630.333333333334</v>
+      </c>
       <c r="I24" s="1">
         <v>16399.333333333336</v>
       </c>
@@ -4081,7 +4127,9 @@
       <c r="M24" s="1">
         <v>9284.9999999999982</v>
       </c>
-      <c r="N24" s="1"/>
+      <c r="N24" s="1">
+        <v>23440</v>
+      </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
@@ -4105,7 +4153,9 @@
       <c r="G25" s="1">
         <v>16150.666666666666</v>
       </c>
-      <c r="H25" s="1"/>
+      <c r="H25" s="1">
+        <v>16491.666666666668</v>
+      </c>
       <c r="I25" s="1">
         <v>28602.666666666668</v>
       </c>
@@ -4121,7 +4171,9 @@
       <c r="M25" s="1">
         <v>23870.333333333332</v>
       </c>
-      <c r="N25" s="1"/>
+      <c r="N25" s="1">
+        <v>31176</v>
+      </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
@@ -4284,7 +4336,9 @@
       <c r="G22" s="1">
         <v>80146.333333333328</v>
       </c>
-      <c r="H22" s="1"/>
+      <c r="H22" s="1">
+        <v>79588</v>
+      </c>
       <c r="I22" s="1">
         <v>143408.33333333334</v>
       </c>
@@ -4300,7 +4354,9 @@
       <c r="M22" s="1">
         <v>139288.33333333334</v>
       </c>
-      <c r="N22" s="1"/>
+      <c r="N22" s="1">
+        <v>149700.33333333334</v>
+      </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
@@ -4324,7 +4380,9 @@
       <c r="G23" s="1">
         <v>177506.66666666669</v>
       </c>
-      <c r="H23" s="1"/>
+      <c r="H23" s="1">
+        <v>105545</v>
+      </c>
       <c r="I23" s="1">
         <v>403286</v>
       </c>
@@ -4340,7 +4398,9 @@
       <c r="M23" s="1">
         <v>440149.33333333326</v>
       </c>
-      <c r="N23" s="1"/>
+      <c r="N23" s="1">
+        <v>216158.33333333334</v>
+      </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
@@ -4364,7 +4424,9 @@
       <c r="G24" s="1">
         <v>156733</v>
       </c>
-      <c r="H24" s="1"/>
+      <c r="H24" s="1">
+        <v>346493.66666666663</v>
+      </c>
       <c r="I24" s="1">
         <v>369393.66666666663</v>
       </c>
@@ -4380,7 +4442,9 @@
       <c r="M24" s="1">
         <v>328337</v>
       </c>
-      <c r="N24" s="1"/>
+      <c r="N24" s="1">
+        <v>867790.66666666651</v>
+      </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
@@ -4404,7 +4468,9 @@
       <c r="G25" s="1">
         <v>414386</v>
       </c>
-      <c r="H25" s="1"/>
+      <c r="H25" s="1">
+        <v>531626.66666666663</v>
+      </c>
       <c r="I25" s="1">
         <v>916088</v>
       </c>
@@ -4420,7 +4486,9 @@
       <c r="M25" s="1">
         <v>907774.66666666663</v>
       </c>
-      <c r="N25" s="1"/>
+      <c r="N25" s="1">
+        <v>1233649.3333333333</v>
+      </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>

</xml_diff>